<commit_message>
updated tester and poster
</commit_message>
<xml_diff>
--- a/documentation/MetricScores.xlsx
+++ b/documentation/MetricScores.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/Desktop/MiMic/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F70581-EB7A-794B-88A9-5BDECB4A3FEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73486445-89C7-4A4C-88C0-CF52EC7B569A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1980" windowWidth="28040" windowHeight="17440" xr2:uid="{2B8A1A5E-36EC-B94F-9819-A3C0A9F8D337}"/>
+    <workbookView xWindow="9100" yWindow="2280" windowWidth="28040" windowHeight="17440" xr2:uid="{2B8A1A5E-36EC-B94F-9819-A3C0A9F8D337}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$G$5</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,70 +34,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Mimic (Q&amp;A)</t>
   </si>
   <si>
-    <t>Mimi (Friends)</t>
-  </si>
-  <si>
-    <t>Model B (Q&amp;A)</t>
-  </si>
-  <si>
-    <t>Model B (Friends)</t>
-  </si>
-  <si>
-    <t>BLUE SCORE</t>
-  </si>
-  <si>
-    <t>ROGUE-1 Recall</t>
-  </si>
-  <si>
-    <t>ROGUE-1 Precision</t>
-  </si>
-  <si>
-    <t>ROGUE-1 F1</t>
-  </si>
-  <si>
-    <t>ROGUE-l Recall</t>
-  </si>
-  <si>
-    <t>ROGUE-l Precision</t>
-  </si>
-  <si>
-    <t>ROGUE-l F1</t>
-  </si>
-  <si>
-    <t>METEOR Precision</t>
-  </si>
-  <si>
-    <t>METEOR Recall</t>
-  </si>
-  <si>
-    <t>METEOR F1</t>
-  </si>
-  <si>
-    <t>METEOR Score</t>
-  </si>
-  <si>
-    <t>WER Average</t>
-  </si>
-  <si>
-    <t>Human Average Score</t>
-  </si>
-  <si>
-    <t>METEOR fmean</t>
-  </si>
-  <si>
-    <t>Metric Name</t>
+    <t>Metric:</t>
+  </si>
+  <si>
+    <t>Mimic (Joey)</t>
+  </si>
+  <si>
+    <t>Transform (Q&amp;A)</t>
+  </si>
+  <si>
+    <t>Transform (Joey)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>BLEU:</t>
+  </si>
+  <si>
+    <t>ROUGE-1:</t>
+  </si>
+  <si>
+    <t>METEOR:</t>
+  </si>
+  <si>
+    <t>Human:</t>
+  </si>
+  <si>
+    <r>
+      <t>ROUGE-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>WER Average:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,36 +112,41 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <i/>
-      <sz val="12"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -148,17 +161,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -185,15 +187,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,208 +512,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C84827F-8003-1948-89AC-1DB13759461E}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>18</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="4">
+        <v>5.5334819988161997E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.22287666004090601</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.2125318324547</v>
+      </c>
+      <c r="E2" s="4">
+        <v>8.8011092835394905E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.88030423280423198</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B3" s="4">
+        <v>4.2827845753402099E-3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.136149803158956</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.117777333523328</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5.3232871439826801E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.1593374060150301</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0.06</v>
-      </c>
-      <c r="C2">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.04</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0.17</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0.04</v>
-      </c>
-      <c r="C6">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>0.17</v>
-      </c>
-      <c r="C7">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0.05</v>
-      </c>
-      <c r="C8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0.12</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.22</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.18</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0.13</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="C12" s="7">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.09</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0.06</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>1.97</v>
-      </c>
-      <c r="C14">
-        <v>3.08</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>